<commit_message>
Recursos tentativos de eliminar
Recursos tentativos de eliminar
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion14/escaleta_CN_10_14_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion14/escaleta_CN_10_14_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion14\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -841,7 +846,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,6 +919,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -970,7 +981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1041,16 +1052,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1092,24 +1121,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,7 +1157,7 @@
       <sheetName val="DATOS"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
@@ -1185,7 +1207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1220,7 +1242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,9 +1453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V43" sqref="V43"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,94 +1484,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="T1" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="U1" s="38" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="45"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="51"/>
       <c r="M2" s="19" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="54"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1884,60 +1906,60 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="21" t="s">
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="61">
         <v>5</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="N10" s="7"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23" t="s">
+      <c r="N10" s="62"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="24">
+      <c r="Q10" s="60">
         <v>6</v>
       </c>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="T10" s="26" t="s">
+      <c r="T10" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="U10" s="60" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2467,62 +2489,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="21" t="s">
+      <c r="F23" s="60"/>
+      <c r="G23" s="60" t="s">
         <v>231</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="61">
         <v>11</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7" t="s">
+      <c r="M23" s="62"/>
+      <c r="N23" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23" t="s">
+      <c r="O23" s="60"/>
+      <c r="P23" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="24">
+      <c r="Q23" s="60">
         <v>6</v>
       </c>
-      <c r="R23" s="25" t="s">
+      <c r="R23" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="S23" s="24" t="s">
+      <c r="S23" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="T23" s="26" t="s">
+      <c r="T23" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="U23" s="24" t="s">
+      <c r="U23" s="60" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2758,62 +2780,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="60" t="s">
         <v>233</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="21" t="s">
+      <c r="F28" s="60"/>
+      <c r="G28" s="60" t="s">
         <v>235</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="61">
         <v>16</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7" t="s">
+      <c r="M28" s="62"/>
+      <c r="N28" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23" t="s">
+      <c r="O28" s="60"/>
+      <c r="P28" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="24">
+      <c r="Q28" s="60">
         <v>6</v>
       </c>
-      <c r="R28" s="25" t="s">
+      <c r="R28" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="S28" s="24" t="s">
+      <c r="S28" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="T28" s="26" t="s">
+      <c r="T28" s="60" t="s">
         <v>206</v>
       </c>
-      <c r="U28" s="24" t="s">
+      <c r="U28" s="60" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3058,62 +3080,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="21" t="s">
+      <c r="F34" s="60"/>
+      <c r="G34" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="61">
         <v>20</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="J34" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K34" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L34" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7" t="s">
+      <c r="M34" s="62"/>
+      <c r="N34" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23" t="s">
+      <c r="O34" s="60"/>
+      <c r="P34" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="24">
+      <c r="Q34" s="60">
         <v>6</v>
       </c>
-      <c r="R34" s="25" t="s">
+      <c r="R34" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="S34" s="24" t="s">
+      <c r="S34" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="T34" s="26" t="s">
+      <c r="T34" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="U34" s="24" t="s">
+      <c r="U34" s="60" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4982,12 +5004,6 @@
     <row r="298" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5002,6 +5018,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Eliminación de más recursos
Eliminación de más recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion14/escaleta_CN_10_14_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion14/escaleta_CN_10_14_CO.xlsx
@@ -1052,34 +1052,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,17 +1114,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1453,9 +1453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,94 +1484,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="51"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="19" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="39"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="59"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1906,60 +1906,60 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+    <row r="10" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="H10" s="61">
+      <c r="H10" s="38">
         <v>5</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="K10" s="62" t="s">
+      <c r="K10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="62" t="s">
+      <c r="L10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="62" t="s">
+      <c r="M10" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N10" s="62"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60" t="s">
+      <c r="N10" s="39"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="60">
+      <c r="Q10" s="37">
         <v>6</v>
       </c>
-      <c r="R10" s="60" t="s">
+      <c r="R10" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="S10" s="60" t="s">
+      <c r="S10" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="T10" s="60" t="s">
+      <c r="T10" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="U10" s="60" t="s">
+      <c r="U10" s="37" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2430,121 +2430,121 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="21" t="s">
+      <c r="F22" s="37"/>
+      <c r="G22" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="38">
         <v>10</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7" t="s">
+      <c r="M22" s="39"/>
+      <c r="N22" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23" t="s">
+      <c r="O22" s="37"/>
+      <c r="P22" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="24">
+      <c r="Q22" s="37">
         <v>6</v>
       </c>
-      <c r="R22" s="25" t="s">
+      <c r="R22" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S22" s="24" t="s">
+      <c r="S22" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T22" s="26" t="s">
+      <c r="T22" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="U22" s="24" t="s">
+      <c r="U22" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="59" t="s">
+    <row r="23" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60" t="s">
+      <c r="F23" s="37"/>
+      <c r="G23" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="H23" s="61">
+      <c r="H23" s="38">
         <v>11</v>
       </c>
-      <c r="I23" s="62" t="s">
+      <c r="I23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="K23" s="62" t="s">
+      <c r="K23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="62" t="s">
+      <c r="L23" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62" t="s">
+      <c r="M23" s="39"/>
+      <c r="N23" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60" t="s">
+      <c r="O23" s="37"/>
+      <c r="P23" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="60">
+      <c r="Q23" s="37">
         <v>6</v>
       </c>
-      <c r="R23" s="60" t="s">
+      <c r="R23" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S23" s="60" t="s">
+      <c r="S23" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T23" s="60" t="s">
+      <c r="T23" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="U23" s="60" t="s">
+      <c r="U23" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2721,121 +2721,121 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="21" t="s">
+      <c r="F27" s="37"/>
+      <c r="G27" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="38">
         <v>15</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7" t="s">
+      <c r="M27" s="39"/>
+      <c r="N27" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23" t="s">
+      <c r="O27" s="37"/>
+      <c r="P27" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="24">
+      <c r="Q27" s="37">
         <v>6</v>
       </c>
-      <c r="R27" s="25" t="s">
+      <c r="R27" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S27" s="24" t="s">
+      <c r="S27" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T27" s="26" t="s">
+      <c r="T27" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="U27" s="24" t="s">
+      <c r="U27" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
+    <row r="28" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="E28" s="60" t="s">
+      <c r="E28" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60" t="s">
+      <c r="F28" s="37"/>
+      <c r="G28" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="H28" s="61">
+      <c r="H28" s="38">
         <v>16</v>
       </c>
-      <c r="I28" s="62" t="s">
+      <c r="I28" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="60" t="s">
+      <c r="J28" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="K28" s="62" t="s">
+      <c r="K28" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="62" t="s">
+      <c r="L28" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62" t="s">
+      <c r="M28" s="39"/>
+      <c r="N28" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60" t="s">
+      <c r="O28" s="37"/>
+      <c r="P28" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="60">
+      <c r="Q28" s="37">
         <v>6</v>
       </c>
-      <c r="R28" s="60" t="s">
+      <c r="R28" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S28" s="60" t="s">
+      <c r="S28" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T28" s="60" t="s">
+      <c r="T28" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="U28" s="60" t="s">
+      <c r="U28" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3080,62 +3080,62 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="63" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="59" t="s">
+    <row r="34" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="E34" s="60" t="s">
+      <c r="E34" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60" t="s">
+      <c r="F34" s="37"/>
+      <c r="G34" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="H34" s="61">
+      <c r="H34" s="38">
         <v>20</v>
       </c>
-      <c r="I34" s="62" t="s">
+      <c r="I34" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="60" t="s">
+      <c r="J34" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="K34" s="62" t="s">
+      <c r="K34" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="62" t="s">
+      <c r="L34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62" t="s">
+      <c r="M34" s="39"/>
+      <c r="N34" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="60"/>
-      <c r="P34" s="60" t="s">
+      <c r="O34" s="37"/>
+      <c r="P34" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="60">
+      <c r="Q34" s="37">
         <v>6</v>
       </c>
-      <c r="R34" s="60" t="s">
+      <c r="R34" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S34" s="60" t="s">
+      <c r="S34" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T34" s="60" t="s">
+      <c r="T34" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="U34" s="60" t="s">
+      <c r="U34" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3198,60 +3198,60 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="21" t="s">
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="H36" s="17">
+      <c r="H36" s="38">
         <v>22</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J36" s="22" t="s">
+      <c r="J36" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M36" s="7" t="s">
+      <c r="M36" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N36" s="7"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23" t="s">
+      <c r="N36" s="39"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="24">
+      <c r="Q36" s="37">
         <v>6</v>
       </c>
-      <c r="R36" s="25" t="s">
+      <c r="R36" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="S36" s="24" t="s">
+      <c r="S36" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="T36" s="26" t="s">
+      <c r="T36" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="U36" s="24" t="s">
+      <c r="U36" s="37" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3380,117 +3380,117 @@
         <v>252</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+    <row r="40" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="21" t="s">
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="36">
         <v>24</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="22" t="s">
+      <c r="J40" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="K40" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L40" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7" t="s">
+      <c r="M40" s="39"/>
+      <c r="N40" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23" t="s">
+      <c r="O40" s="37"/>
+      <c r="P40" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q40" s="24">
+      <c r="Q40" s="37">
         <v>6</v>
       </c>
-      <c r="R40" s="25" t="s">
+      <c r="R40" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S40" s="24" t="s">
+      <c r="S40" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T40" s="26" t="s">
+      <c r="T40" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="U40" s="24" t="s">
+      <c r="U40" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="21" t="s">
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="36">
         <v>25</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="22" t="s">
+      <c r="J41" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="K41" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="L41" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7" t="s">
+      <c r="M41" s="39"/>
+      <c r="N41" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23" t="s">
+      <c r="O41" s="37"/>
+      <c r="P41" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q41" s="24">
+      <c r="Q41" s="37">
         <v>6</v>
       </c>
-      <c r="R41" s="25" t="s">
+      <c r="R41" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S41" s="24" t="s">
+      <c r="S41" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T41" s="26" t="s">
+      <c r="T41" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="U41" s="24" t="s">
+      <c r="U41" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3551,60 +3551,60 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="21" t="s">
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="36">
         <v>27</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J43" s="22" t="s">
+      <c r="J43" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="K43" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7" t="s">
+      <c r="M43" s="39"/>
+      <c r="N43" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23" t="s">
+      <c r="O43" s="37"/>
+      <c r="P43" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q43" s="24">
+      <c r="Q43" s="37">
         <v>6</v>
       </c>
-      <c r="R43" s="25" t="s">
+      <c r="R43" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="S43" s="24" t="s">
+      <c r="S43" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="T43" s="26" t="s">
+      <c r="T43" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="U43" s="24" t="s">
+      <c r="U43" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5004,6 +5004,12 @@
     <row r="298" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5018,12 +5024,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>